<commit_message>
refs #662, Revision Changes; bug with creatives
</commit_message>
<xml_diff>
--- a/spec/fixtures/io_files/Collective_IO_revised_new_lis.xlsx
+++ b/spec/fixtures/io_files/Collective_IO_revised_new_lis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Insertion Order" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,6 +28,9 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
@@ -37,6 +40,9 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
@@ -46,13 +52,16 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="176">
   <si>
     <t>Date:</t>
   </si>
@@ -600,7 +609,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="M/D/YYYY" numFmtId="165"/>
     <numFmt formatCode="\$#,##0.00" numFmtId="166"/>
@@ -608,9 +617,10 @@
     <numFmt formatCode="\$#,##0.00_);[RED]&quot;($&quot;#,##0.00\)" numFmtId="168"/>
     <numFmt formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)" numFmtId="169"/>
     <numFmt formatCode="\$#,##0.00_);&quot;($&quot;#,##0.00\)" numFmtId="170"/>
-    <numFmt formatCode="@" numFmtId="171"/>
+    <numFmt formatCode="MM/DD/YY" numFmtId="171"/>
+    <numFmt formatCode="@" numFmtId="172"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="28">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -752,6 +762,18 @@
       <charset val="1"/>
       <family val="2"/>
       <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
       <sz val="11"/>
       <u val="single"/>
     </font>
@@ -960,7 +982,7 @@
       <protection hidden="false" locked="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="128">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -1337,11 +1359,23 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="21" numFmtId="171" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="20" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="21">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="21" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="23" numFmtId="164" xfId="21">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1365,7 +1399,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="22" numFmtId="164" xfId="21">
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="24" numFmtId="164" xfId="21">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1377,35 +1411,35 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="25" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="25" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="25" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="25" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="24" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="26" numFmtId="164" xfId="20">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="25" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="27" numFmtId="164" xfId="20">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="2" fontId="22" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="2" fontId="24" numFmtId="164" xfId="21">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="22" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="24" numFmtId="164" xfId="21">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1421,27 +1455,27 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="23" numFmtId="171" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="25" numFmtId="172" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="3" fillId="2" fontId="24" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="3" fillId="2" fontId="26" numFmtId="164" xfId="20">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="13" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="13" fillId="2" fontId="25" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="13" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="13" fillId="2" fontId="25" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="21" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="23" numFmtId="164" xfId="21">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="21" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="23" numFmtId="164" xfId="21">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1449,15 +1483,15 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="2" fontId="25" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="23" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="25" numFmtId="164" xfId="20">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="2" fontId="25" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1470,7 +1504,7 @@
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
     <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="21"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="21"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1540,15 +1574,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>347760</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>4680</xdr:rowOff>
+      <xdr:colOff>428760</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>25200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>578160</xdr:colOff>
+      <xdr:colOff>658080</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>48960</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1563,8 +1597,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="347760" y="147240"/>
-          <a:ext cx="1228320" cy="596880"/>
+          <a:off x="428760" y="120240"/>
+          <a:ext cx="1227240" cy="595800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1576,15 +1610,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>324000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>117720</xdr:colOff>
+      <xdr:colOff>197640</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:rowOff>46800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1593,8 +1627,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="243000" y="3600"/>
-          <a:ext cx="12352320" cy="44280"/>
+          <a:off x="324000" y="3600"/>
+          <a:ext cx="12351240" cy="43200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1615,15 +1649,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>324000</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>119160</xdr:rowOff>
+      <xdr:rowOff>92160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>117720</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:colOff>197640</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>135360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1632,8 +1666,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="243000" y="814320"/>
-          <a:ext cx="12352320" cy="44280"/>
+          <a:off x="324000" y="787320"/>
+          <a:ext cx="12351240" cy="43200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1654,15 +1688,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>324000</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>106200</xdr:rowOff>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>155880</xdr:colOff>
+      <xdr:colOff>235800</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>84240</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1671,8 +1705,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="243000" y="6146280"/>
-          <a:ext cx="12390480" cy="139680"/>
+          <a:off x="324000" y="6119280"/>
+          <a:ext cx="12389400" cy="138600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1693,15 +1727,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>324000</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>146520</xdr:colOff>
+      <xdr:colOff>226440</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>101520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1710,8 +1744,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="243000" y="2900160"/>
-          <a:ext cx="12381120" cy="42480"/>
+          <a:off x="324000" y="2873160"/>
+          <a:ext cx="12380040" cy="41400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1737,15 +1771,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>300240</xdr:colOff>
+      <xdr:colOff>381240</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>3240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>363600</xdr:colOff>
+      <xdr:colOff>443520</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>200160</xdr:rowOff>
+      <xdr:rowOff>199080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1760,8 +1794,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="300240" y="3240"/>
-          <a:ext cx="1594800" cy="720720"/>
+          <a:off x="381240" y="3240"/>
+          <a:ext cx="1593720" cy="719640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1778,15 +1812,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>347760</xdr:colOff>
+      <xdr:colOff>428760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>33480</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>411120</xdr:colOff>
+      <xdr:colOff>491040</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>230400</xdr:rowOff>
+      <xdr:rowOff>202320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1801,8 +1835,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="347760" y="33480"/>
-          <a:ext cx="1594800" cy="720720"/>
+          <a:off x="428760" y="6480"/>
+          <a:ext cx="1593720" cy="719640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1819,15 +1853,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>347760</xdr:colOff>
+      <xdr:colOff>428760</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>411120</xdr:colOff>
+      <xdr:colOff>491040</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>200520</xdr:rowOff>
+      <xdr:rowOff>199440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1842,8 +1876,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="347760" y="3600"/>
-          <a:ext cx="1594800" cy="720720"/>
+          <a:off x="428760" y="3600"/>
+          <a:ext cx="1593720" cy="719640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1862,8 +1896,8 @@
   </sheetPr>
   <dimension ref="A1:AI181"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D30" activeCellId="0" pane="topLeft" sqref="D30"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A31" activeCellId="0" pane="topLeft" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4514,8 +4548,8 @@
   </sheetPr>
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="I4" activeCellId="0" pane="topLeft" sqref="I4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="E1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="J11" activeCellId="0" pane="topLeft" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4838,12 +4872,62 @@
         <v>http://ad.doubleclick.net/jump/.collective;adid=;sz=160x600</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
+      <c r="A10" s="91" t="str">
+        <f aca="false">'Insertion Order'!C18</f>
+        <v>Otterbein University</v>
+      </c>
+      <c r="G10" s="91" t="str">
+        <f aca="false">'Insertion Order'!D31</f>
+        <v>Test New LI</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="94" t="n">
+        <v>41731</v>
+      </c>
+      <c r="J10" s="94" t="n">
+        <v>41743</v>
+      </c>
+      <c r="K10" s="95" t="str">
+        <f aca="false">CONCATENATE(B9,C9,E9,F9,H9)</f>
+        <v>http://ad.doubleclick.net/ad/.collective;adid=;sz=160x600</v>
+      </c>
+      <c r="L10" s="96" t="str">
+        <f aca="false">CONCATENATE(B9,D9,E9,F9,H9)</f>
+        <v>http://ad.doubleclick.net/jump/.collective;adid=;sz=160x600</v>
+      </c>
       <c r="R10" s="88" t="s">
         <v>86</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
+      <c r="A11" s="91" t="str">
+        <f aca="false">'Insertion Order'!C18</f>
+        <v>Otterbein University</v>
+      </c>
+      <c r="G11" s="91" t="str">
+        <f aca="false">'Insertion Order'!D32</f>
+        <v>Test New LI #2</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="94" t="n">
+        <v>41731</v>
+      </c>
+      <c r="J11" s="94" t="n">
+        <v>41743</v>
+      </c>
+      <c r="K11" s="95" t="str">
+        <f aca="false">CONCATENATE(B9,C9,E9,F9,H9)</f>
+        <v>http://ad.doubleclick.net/ad/.collective;adid=;sz=160x600</v>
+      </c>
+      <c r="L11" s="95" t="str">
+        <f aca="false">CONCATENATE(B9,D9,E9,F9,H9)</f>
+        <v>http://ad.doubleclick.net/jump/.collective;adid=;sz=160x600</v>
+      </c>
       <c r="R11" s="89" t="s">
         <v>48</v>
       </c>
@@ -4912,368 +4996,368 @@
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
-      <c r="C3" s="94"/>
-      <c r="D3" s="95" t="s">
+      <c r="C3" s="97"/>
+      <c r="D3" s="98" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="I3" s="96"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="I3" s="99"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="26.1" outlineLevel="0" r="4"/>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39" outlineLevel="0" r="5" s="100">
-      <c r="A5" s="97" t="s">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39" outlineLevel="0" r="5" s="103">
+      <c r="A5" s="100" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="97" t="s">
+      <c r="C5" s="100" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="100" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="100" t="s">
         <v>91</v>
       </c>
-      <c r="F5" s="97" t="s">
+      <c r="F5" s="100" t="s">
         <v>92</v>
       </c>
-      <c r="G5" s="97" t="s">
+      <c r="G5" s="100" t="s">
         <v>93</v>
       </c>
-      <c r="H5" s="98" t="s">
+      <c r="H5" s="101" t="s">
         <v>94</v>
       </c>
-      <c r="I5" s="97" t="s">
+      <c r="I5" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="J5" s="97" t="s">
+      <c r="J5" s="100" t="s">
         <v>96</v>
       </c>
-      <c r="K5" s="97" t="s">
+      <c r="K5" s="100" t="s">
         <v>97</v>
       </c>
-      <c r="L5" s="97" t="s">
+      <c r="L5" s="100" t="s">
         <v>98</v>
       </c>
-      <c r="M5" s="98" t="s">
+      <c r="M5" s="101" t="s">
         <v>99</v>
       </c>
-      <c r="N5" s="98" t="s">
+      <c r="N5" s="101" t="s">
         <v>100</v>
       </c>
-      <c r="O5" s="98" t="s">
+      <c r="O5" s="101" t="s">
         <v>101</v>
       </c>
-      <c r="P5" s="98" t="s">
+      <c r="P5" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="Q5" s="97" t="s">
+      <c r="Q5" s="100" t="s">
         <v>103</v>
       </c>
-      <c r="R5" s="99"/>
+      <c r="R5" s="102"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
-      <c r="A6" s="101"/>
-      <c r="B6" s="102"/>
-      <c r="C6" s="102"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="102"/>
-      <c r="I6" s="102"/>
-      <c r="J6" s="102"/>
-      <c r="K6" s="102"/>
-      <c r="L6" s="102"/>
-      <c r="M6" s="102"/>
-      <c r="N6" s="102"/>
-      <c r="O6" s="102"/>
-      <c r="P6" s="102"/>
-      <c r="Q6" s="102"/>
-      <c r="R6" s="103"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="111">
-      <c r="A7" s="104" t="s">
+      <c r="A6" s="104"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="105"/>
+      <c r="J6" s="105"/>
+      <c r="K6" s="105"/>
+      <c r="L6" s="105"/>
+      <c r="M6" s="105"/>
+      <c r="N6" s="105"/>
+      <c r="O6" s="105"/>
+      <c r="P6" s="105"/>
+      <c r="Q6" s="105"/>
+      <c r="R6" s="106"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="114">
+      <c r="A7" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="104" t="s">
+      <c r="B7" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="105" t="s">
+      <c r="C7" s="108" t="s">
         <v>106</v>
       </c>
-      <c r="D7" s="104" t="s">
+      <c r="D7" s="107" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="104" t="s">
+      <c r="E7" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="F7" s="104" t="s">
+      <c r="F7" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="G7" s="105" t="s">
+      <c r="G7" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="H7" s="106" t="n">
+      <c r="H7" s="109" t="n">
         <v>8</v>
       </c>
-      <c r="I7" s="105" t="s">
+      <c r="I7" s="108" t="s">
         <v>110</v>
       </c>
-      <c r="J7" s="105" t="s">
+      <c r="J7" s="108" t="s">
         <v>111</v>
       </c>
-      <c r="K7" s="104" t="s">
+      <c r="K7" s="107" t="s">
         <v>112</v>
       </c>
-      <c r="L7" s="104" t="s">
+      <c r="L7" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="M7" s="106" t="n">
+      <c r="M7" s="109" t="n">
         <v>20</v>
       </c>
-      <c r="N7" s="107" t="s">
+      <c r="N7" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="O7" s="106" t="s">
+      <c r="O7" s="109" t="s">
         <v>115</v>
       </c>
-      <c r="P7" s="108" t="s">
+      <c r="P7" s="111" t="s">
         <v>116</v>
       </c>
-      <c r="Q7" s="109"/>
-      <c r="R7" s="110"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="8" s="111">
-      <c r="A8" s="104" t="s">
+      <c r="Q7" s="112"/>
+      <c r="R7" s="113"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="8" s="114">
+      <c r="A8" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="105" t="s">
+      <c r="C8" s="108" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="104" t="s">
+      <c r="D8" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="104" t="s">
+      <c r="E8" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="F8" s="104" t="s">
+      <c r="F8" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="G8" s="105" t="s">
+      <c r="G8" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="H8" s="106" t="n">
+      <c r="H8" s="109" t="n">
         <v>8</v>
       </c>
-      <c r="I8" s="105" t="s">
+      <c r="I8" s="108" t="s">
         <v>110</v>
       </c>
-      <c r="J8" s="105" t="s">
+      <c r="J8" s="108" t="s">
         <v>111</v>
       </c>
-      <c r="K8" s="104" t="s">
+      <c r="K8" s="107" t="s">
         <v>112</v>
       </c>
-      <c r="L8" s="104" t="s">
+      <c r="L8" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="M8" s="106" t="n">
+      <c r="M8" s="109" t="n">
         <v>20</v>
       </c>
-      <c r="N8" s="107" t="s">
+      <c r="N8" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="O8" s="106" t="s">
+      <c r="O8" s="109" t="s">
         <v>115</v>
       </c>
-      <c r="P8" s="108" t="s">
+      <c r="P8" s="111" t="s">
         <v>116</v>
       </c>
-      <c r="Q8" s="109"/>
-      <c r="R8" s="110"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="9" s="111">
-      <c r="A9" s="104" t="s">
+      <c r="Q8" s="112"/>
+      <c r="R8" s="113"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="9" s="114">
+      <c r="A9" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="104" t="s">
+      <c r="B9" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="105" t="s">
+      <c r="C9" s="108" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="104" t="s">
+      <c r="D9" s="107" t="s">
         <v>119</v>
       </c>
-      <c r="E9" s="104" t="s">
+      <c r="E9" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="F9" s="104" t="s">
+      <c r="F9" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="G9" s="105" t="s">
+      <c r="G9" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="H9" s="106" t="n">
+      <c r="H9" s="109" t="n">
         <v>8</v>
       </c>
-      <c r="I9" s="105" t="s">
+      <c r="I9" s="108" t="s">
         <v>110</v>
       </c>
-      <c r="J9" s="105" t="s">
+      <c r="J9" s="108" t="s">
         <v>111</v>
       </c>
-      <c r="K9" s="104" t="s">
+      <c r="K9" s="107" t="s">
         <v>112</v>
       </c>
-      <c r="L9" s="104" t="s">
+      <c r="L9" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="M9" s="106" t="n">
+      <c r="M9" s="109" t="n">
         <v>20</v>
       </c>
-      <c r="N9" s="107" t="s">
+      <c r="N9" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="O9" s="106" t="s">
+      <c r="O9" s="109" t="s">
         <v>115</v>
       </c>
-      <c r="P9" s="108" t="s">
+      <c r="P9" s="111" t="s">
         <v>116</v>
       </c>
-      <c r="Q9" s="109"/>
-      <c r="R9" s="110"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="10" s="111">
-      <c r="A10" s="104" t="s">
+      <c r="Q9" s="112"/>
+      <c r="R9" s="113"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="10" s="114">
+      <c r="A10" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="104" t="s">
+      <c r="B10" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="105" t="s">
+      <c r="C10" s="108" t="s">
         <v>120</v>
       </c>
-      <c r="D10" s="104" t="s">
+      <c r="D10" s="107" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="104" t="s">
+      <c r="E10" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="F10" s="104" t="s">
+      <c r="F10" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="G10" s="105" t="s">
+      <c r="G10" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="H10" s="106" t="n">
+      <c r="H10" s="109" t="n">
         <v>8</v>
       </c>
-      <c r="I10" s="105" t="s">
+      <c r="I10" s="108" t="s">
         <v>110</v>
       </c>
-      <c r="J10" s="105" t="s">
+      <c r="J10" s="108" t="s">
         <v>111</v>
       </c>
-      <c r="K10" s="104" t="s">
+      <c r="K10" s="107" t="s">
         <v>112</v>
       </c>
-      <c r="L10" s="104" t="s">
+      <c r="L10" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="M10" s="106" t="n">
+      <c r="M10" s="109" t="n">
         <v>20</v>
       </c>
-      <c r="N10" s="107" t="s">
+      <c r="N10" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="O10" s="106" t="s">
+      <c r="O10" s="109" t="s">
         <v>115</v>
       </c>
-      <c r="P10" s="108" t="s">
+      <c r="P10" s="111" t="s">
         <v>116</v>
       </c>
-      <c r="Q10" s="109"/>
-      <c r="R10" s="110"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="11" s="111">
-      <c r="A11" s="104" t="s">
+      <c r="Q10" s="112"/>
+      <c r="R10" s="113"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="11" s="114">
+      <c r="A11" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="104" t="s">
+      <c r="B11" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="105" t="s">
+      <c r="C11" s="108" t="s">
         <v>121</v>
       </c>
-      <c r="D11" s="104" t="s">
+      <c r="D11" s="107" t="s">
         <v>122</v>
       </c>
-      <c r="E11" s="104" t="s">
+      <c r="E11" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="F11" s="104" t="s">
+      <c r="F11" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="G11" s="105" t="s">
+      <c r="G11" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="H11" s="106" t="n">
+      <c r="H11" s="109" t="n">
         <v>8</v>
       </c>
-      <c r="I11" s="105" t="s">
+      <c r="I11" s="108" t="s">
         <v>110</v>
       </c>
-      <c r="J11" s="105" t="s">
+      <c r="J11" s="108" t="s">
         <v>111</v>
       </c>
-      <c r="K11" s="104" t="s">
+      <c r="K11" s="107" t="s">
         <v>112</v>
       </c>
-      <c r="L11" s="104" t="s">
+      <c r="L11" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="M11" s="106" t="n">
+      <c r="M11" s="109" t="n">
         <v>20</v>
       </c>
-      <c r="N11" s="107" t="s">
+      <c r="N11" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="O11" s="106" t="s">
+      <c r="O11" s="109" t="s">
         <v>115</v>
       </c>
-      <c r="P11" s="108" t="s">
+      <c r="P11" s="111" t="s">
         <v>116</v>
       </c>
-      <c r="Q11" s="109"/>
-      <c r="R11" s="110"/>
+      <c r="Q11" s="112"/>
+      <c r="R11" s="113"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.5" outlineLevel="0" r="12">
-      <c r="A12" s="112"/>
-      <c r="B12" s="113"/>
-      <c r="C12" s="113"/>
-      <c r="D12" s="113"/>
-      <c r="E12" s="113"/>
-      <c r="F12" s="113"/>
-      <c r="G12" s="113"/>
-      <c r="H12" s="113"/>
-      <c r="I12" s="113"/>
-      <c r="J12" s="113"/>
-      <c r="K12" s="113"/>
-      <c r="L12" s="113"/>
-      <c r="M12" s="113"/>
-      <c r="N12" s="113"/>
-      <c r="O12" s="113"/>
-      <c r="P12" s="113"/>
-      <c r="Q12" s="113"/>
-      <c r="R12" s="114"/>
+      <c r="A12" s="115"/>
+      <c r="B12" s="116"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="116"/>
+      <c r="H12" s="116"/>
+      <c r="I12" s="116"/>
+      <c r="J12" s="116"/>
+      <c r="K12" s="116"/>
+      <c r="L12" s="116"/>
+      <c r="M12" s="116"/>
+      <c r="N12" s="116"/>
+      <c r="O12" s="116"/>
+      <c r="P12" s="116"/>
+      <c r="Q12" s="116"/>
+      <c r="R12" s="117"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5325,545 +5409,545 @@
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
-      <c r="C3" s="94"/>
-      <c r="D3" s="95" t="s">
+      <c r="C3" s="97"/>
+      <c r="D3" s="98" t="s">
         <v>123</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="4"/>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="51.75" outlineLevel="0" r="5" s="100">
-      <c r="A5" s="97" t="s">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="51.75" outlineLevel="0" r="5" s="103">
+      <c r="A5" s="100" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="97" t="s">
+      <c r="C5" s="100" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="100" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="100" t="s">
         <v>124</v>
       </c>
-      <c r="F5" s="97" t="s">
+      <c r="F5" s="100" t="s">
         <v>125</v>
       </c>
-      <c r="G5" s="97" t="s">
+      <c r="G5" s="100" t="s">
         <v>126</v>
       </c>
-      <c r="H5" s="97" t="s">
+      <c r="H5" s="100" t="s">
         <v>127</v>
       </c>
-      <c r="I5" s="97" t="s">
+      <c r="I5" s="100" t="s">
         <v>93</v>
       </c>
-      <c r="J5" s="98" t="s">
+      <c r="J5" s="101" t="s">
         <v>94</v>
       </c>
-      <c r="K5" s="97" t="s">
+      <c r="K5" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="L5" s="97" t="s">
+      <c r="L5" s="100" t="s">
         <v>97</v>
       </c>
-      <c r="M5" s="97" t="s">
+      <c r="M5" s="100" t="s">
         <v>98</v>
       </c>
-      <c r="N5" s="98" t="s">
+      <c r="N5" s="101" t="s">
         <v>99</v>
       </c>
-      <c r="O5" s="98" t="s">
+      <c r="O5" s="101" t="s">
         <v>128</v>
       </c>
-      <c r="P5" s="98" t="s">
+      <c r="P5" s="101" t="s">
         <v>129</v>
       </c>
-      <c r="Q5" s="98" t="s">
+      <c r="Q5" s="101" t="s">
         <v>130</v>
       </c>
-      <c r="R5" s="98" t="s">
+      <c r="R5" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="S5" s="98" t="s">
+      <c r="S5" s="101" t="s">
         <v>132</v>
       </c>
-      <c r="T5" s="98" t="s">
+      <c r="T5" s="101" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="98" t="s">
+      <c r="U5" s="101" t="s">
         <v>134</v>
       </c>
-      <c r="V5" s="97" t="s">
+      <c r="V5" s="100" t="s">
         <v>135</v>
       </c>
-      <c r="W5" s="98" t="s">
+      <c r="W5" s="101" t="s">
         <v>136</v>
       </c>
-      <c r="X5" s="98" t="s">
+      <c r="X5" s="101" t="s">
         <v>101</v>
       </c>
-      <c r="Y5" s="98" t="s">
+      <c r="Y5" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="Z5" s="97" t="s">
+      <c r="Z5" s="100" t="s">
         <v>103</v>
       </c>
-      <c r="AA5" s="99"/>
+      <c r="AA5" s="102"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
-      <c r="A6" s="101"/>
-      <c r="B6" s="102"/>
-      <c r="C6" s="102"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="102"/>
-      <c r="I6" s="102"/>
-      <c r="J6" s="102"/>
-      <c r="K6" s="102"/>
-      <c r="L6" s="102"/>
-      <c r="M6" s="102"/>
-      <c r="N6" s="102"/>
-      <c r="O6" s="102"/>
-      <c r="P6" s="102"/>
-      <c r="Q6" s="102"/>
-      <c r="R6" s="102"/>
-      <c r="S6" s="102"/>
-      <c r="T6" s="102"/>
-      <c r="U6" s="102"/>
-      <c r="V6" s="102"/>
-      <c r="W6" s="102"/>
-      <c r="X6" s="102"/>
-      <c r="Y6" s="102"/>
-      <c r="Z6" s="102"/>
-      <c r="AA6" s="103"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="111">
-      <c r="A7" s="104" t="s">
+      <c r="A6" s="104"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="105"/>
+      <c r="J6" s="105"/>
+      <c r="K6" s="105"/>
+      <c r="L6" s="105"/>
+      <c r="M6" s="105"/>
+      <c r="N6" s="105"/>
+      <c r="O6" s="105"/>
+      <c r="P6" s="105"/>
+      <c r="Q6" s="105"/>
+      <c r="R6" s="105"/>
+      <c r="S6" s="105"/>
+      <c r="T6" s="105"/>
+      <c r="U6" s="105"/>
+      <c r="V6" s="105"/>
+      <c r="W6" s="105"/>
+      <c r="X6" s="105"/>
+      <c r="Y6" s="105"/>
+      <c r="Z6" s="105"/>
+      <c r="AA6" s="106"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="114">
+      <c r="A7" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="104" t="s">
+      <c r="B7" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="105" t="s">
+      <c r="C7" s="108" t="s">
         <v>106</v>
       </c>
-      <c r="D7" s="104" t="s">
+      <c r="D7" s="107" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="104" t="s">
+      <c r="E7" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="104" t="s">
+      <c r="F7" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="G7" s="104" t="s">
+      <c r="G7" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="H7" s="104" t="s">
+      <c r="H7" s="107" t="s">
         <v>138</v>
       </c>
-      <c r="I7" s="105" t="s">
+      <c r="I7" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="J7" s="106" t="n">
+      <c r="J7" s="109" t="n">
         <v>8</v>
       </c>
-      <c r="K7" s="105" t="s">
+      <c r="K7" s="108" t="s">
         <v>110</v>
       </c>
-      <c r="L7" s="104" t="s">
+      <c r="L7" s="107" t="s">
         <v>112</v>
       </c>
-      <c r="M7" s="104" t="s">
+      <c r="M7" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="N7" s="106" t="n">
+      <c r="N7" s="109" t="n">
         <v>24</v>
       </c>
-      <c r="O7" s="107" t="s">
+      <c r="O7" s="110" t="s">
         <v>139</v>
       </c>
-      <c r="P7" s="106" t="s">
+      <c r="P7" s="109" t="s">
         <v>140</v>
       </c>
-      <c r="Q7" s="107" t="s">
+      <c r="Q7" s="110" t="s">
         <v>141</v>
       </c>
-      <c r="R7" s="107" t="s">
+      <c r="R7" s="110" t="s">
         <v>141</v>
       </c>
-      <c r="S7" s="115" t="s">
+      <c r="S7" s="118" t="s">
         <v>142</v>
       </c>
-      <c r="T7" s="106" t="s">
+      <c r="T7" s="109" t="s">
         <v>143</v>
       </c>
-      <c r="U7" s="106" t="s">
+      <c r="U7" s="109" t="s">
         <v>144</v>
       </c>
-      <c r="V7" s="105" t="s">
+      <c r="V7" s="108" t="s">
         <v>145</v>
       </c>
-      <c r="W7" s="107" t="s">
+      <c r="W7" s="110" t="s">
         <v>146</v>
       </c>
-      <c r="X7" s="106" t="s">
+      <c r="X7" s="109" t="s">
         <v>115</v>
       </c>
-      <c r="Y7" s="116" t="s">
+      <c r="Y7" s="119" t="s">
         <v>116</v>
       </c>
-      <c r="Z7" s="109"/>
-      <c r="AA7" s="110"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="8" s="111">
-      <c r="A8" s="104" t="s">
+      <c r="Z7" s="112"/>
+      <c r="AA7" s="113"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="8" s="114">
+      <c r="A8" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="105" t="s">
+      <c r="C8" s="108" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="104" t="s">
+      <c r="D8" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="104" t="s">
+      <c r="E8" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="104" t="s">
+      <c r="F8" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="G8" s="104" t="s">
+      <c r="G8" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="H8" s="104" t="s">
+      <c r="H8" s="107" t="s">
         <v>138</v>
       </c>
-      <c r="I8" s="105" t="s">
+      <c r="I8" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="J8" s="106" t="n">
+      <c r="J8" s="109" t="n">
         <v>8</v>
       </c>
-      <c r="K8" s="105" t="s">
+      <c r="K8" s="108" t="s">
         <v>110</v>
       </c>
-      <c r="L8" s="104" t="s">
+      <c r="L8" s="107" t="s">
         <v>112</v>
       </c>
-      <c r="M8" s="104" t="s">
+      <c r="M8" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="N8" s="106" t="n">
+      <c r="N8" s="109" t="n">
         <v>24</v>
       </c>
-      <c r="O8" s="107" t="s">
+      <c r="O8" s="110" t="s">
         <v>139</v>
       </c>
-      <c r="P8" s="106" t="s">
+      <c r="P8" s="109" t="s">
         <v>140</v>
       </c>
-      <c r="Q8" s="107" t="s">
+      <c r="Q8" s="110" t="s">
         <v>141</v>
       </c>
-      <c r="R8" s="107" t="s">
+      <c r="R8" s="110" t="s">
         <v>141</v>
       </c>
-      <c r="S8" s="115" t="s">
+      <c r="S8" s="118" t="s">
         <v>142</v>
       </c>
-      <c r="T8" s="106" t="s">
+      <c r="T8" s="109" t="s">
         <v>147</v>
       </c>
-      <c r="U8" s="106" t="s">
+      <c r="U8" s="109" t="s">
         <v>148</v>
       </c>
-      <c r="V8" s="105" t="s">
+      <c r="V8" s="108" t="s">
         <v>145</v>
       </c>
-      <c r="W8" s="107" t="s">
+      <c r="W8" s="110" t="s">
         <v>146</v>
       </c>
-      <c r="X8" s="106" t="s">
+      <c r="X8" s="109" t="s">
         <v>115</v>
       </c>
-      <c r="Y8" s="116" t="s">
+      <c r="Y8" s="119" t="s">
         <v>116</v>
       </c>
-      <c r="Z8" s="109"/>
-      <c r="AA8" s="110"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="9" s="111">
-      <c r="A9" s="104" t="s">
+      <c r="Z8" s="112"/>
+      <c r="AA8" s="113"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="9" s="114">
+      <c r="A9" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="104" t="s">
+      <c r="B9" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="105" t="s">
+      <c r="C9" s="108" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="104" t="s">
+      <c r="D9" s="107" t="s">
         <v>119</v>
       </c>
-      <c r="E9" s="104" t="s">
+      <c r="E9" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="F9" s="104" t="s">
+      <c r="F9" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="G9" s="104" t="s">
+      <c r="G9" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="H9" s="104" t="s">
+      <c r="H9" s="107" t="s">
         <v>138</v>
       </c>
-      <c r="I9" s="105" t="s">
+      <c r="I9" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="J9" s="106" t="n">
+      <c r="J9" s="109" t="n">
         <v>8</v>
       </c>
-      <c r="K9" s="105" t="s">
+      <c r="K9" s="108" t="s">
         <v>110</v>
       </c>
-      <c r="L9" s="104" t="s">
+      <c r="L9" s="107" t="s">
         <v>112</v>
       </c>
-      <c r="M9" s="104" t="s">
+      <c r="M9" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="N9" s="106" t="n">
+      <c r="N9" s="109" t="n">
         <v>24</v>
       </c>
-      <c r="O9" s="107" t="s">
+      <c r="O9" s="110" t="s">
         <v>139</v>
       </c>
-      <c r="P9" s="106" t="s">
+      <c r="P9" s="109" t="s">
         <v>140</v>
       </c>
-      <c r="Q9" s="107" t="s">
+      <c r="Q9" s="110" t="s">
         <v>141</v>
       </c>
-      <c r="R9" s="107" t="s">
+      <c r="R9" s="110" t="s">
         <v>141</v>
       </c>
-      <c r="S9" s="115" t="s">
+      <c r="S9" s="118" t="s">
         <v>142</v>
       </c>
-      <c r="T9" s="106" t="s">
+      <c r="T9" s="109" t="s">
         <v>149</v>
       </c>
-      <c r="U9" s="106" t="s">
+      <c r="U9" s="109" t="s">
         <v>148</v>
       </c>
-      <c r="V9" s="105" t="s">
+      <c r="V9" s="108" t="s">
         <v>145</v>
       </c>
-      <c r="W9" s="107" t="s">
+      <c r="W9" s="110" t="s">
         <v>146</v>
       </c>
-      <c r="X9" s="106" t="s">
+      <c r="X9" s="109" t="s">
         <v>115</v>
       </c>
-      <c r="Y9" s="116" t="s">
+      <c r="Y9" s="119" t="s">
         <v>116</v>
       </c>
-      <c r="Z9" s="109"/>
-      <c r="AA9" s="110"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="10" s="111">
-      <c r="A10" s="104" t="s">
+      <c r="Z9" s="112"/>
+      <c r="AA9" s="113"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="10" s="114">
+      <c r="A10" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="104" t="s">
+      <c r="B10" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="105" t="s">
+      <c r="C10" s="108" t="s">
         <v>120</v>
       </c>
-      <c r="D10" s="104" t="s">
+      <c r="D10" s="107" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="104" t="s">
+      <c r="E10" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="104" t="s">
+      <c r="F10" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="G10" s="104" t="s">
+      <c r="G10" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="H10" s="104" t="s">
+      <c r="H10" s="107" t="s">
         <v>138</v>
       </c>
-      <c r="I10" s="105" t="s">
+      <c r="I10" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="J10" s="106" t="n">
+      <c r="J10" s="109" t="n">
         <v>8</v>
       </c>
-      <c r="K10" s="105" t="s">
+      <c r="K10" s="108" t="s">
         <v>110</v>
       </c>
-      <c r="L10" s="104" t="s">
+      <c r="L10" s="107" t="s">
         <v>112</v>
       </c>
-      <c r="M10" s="104" t="s">
+      <c r="M10" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="N10" s="106" t="n">
+      <c r="N10" s="109" t="n">
         <v>24</v>
       </c>
-      <c r="O10" s="107" t="s">
+      <c r="O10" s="110" t="s">
         <v>139</v>
       </c>
-      <c r="P10" s="106" t="s">
+      <c r="P10" s="109" t="s">
         <v>140</v>
       </c>
-      <c r="Q10" s="107" t="s">
+      <c r="Q10" s="110" t="s">
         <v>141</v>
       </c>
-      <c r="R10" s="107" t="s">
+      <c r="R10" s="110" t="s">
         <v>141</v>
       </c>
-      <c r="S10" s="115" t="s">
+      <c r="S10" s="118" t="s">
         <v>142</v>
       </c>
-      <c r="T10" s="106" t="s">
+      <c r="T10" s="109" t="s">
         <v>150</v>
       </c>
-      <c r="U10" s="106" t="s">
+      <c r="U10" s="109" t="s">
         <v>148</v>
       </c>
-      <c r="V10" s="105" t="s">
+      <c r="V10" s="108" t="s">
         <v>145</v>
       </c>
-      <c r="W10" s="107" t="s">
+      <c r="W10" s="110" t="s">
         <v>146</v>
       </c>
-      <c r="X10" s="106" t="s">
+      <c r="X10" s="109" t="s">
         <v>115</v>
       </c>
-      <c r="Y10" s="116" t="s">
+      <c r="Y10" s="119" t="s">
         <v>116</v>
       </c>
-      <c r="Z10" s="109"/>
-      <c r="AA10" s="110"/>
+      <c r="Z10" s="112"/>
+      <c r="AA10" s="113"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="11">
-      <c r="A11" s="104" t="s">
+      <c r="A11" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="104" t="s">
+      <c r="B11" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="105" t="s">
+      <c r="C11" s="108" t="s">
         <v>121</v>
       </c>
-      <c r="D11" s="104" t="s">
+      <c r="D11" s="107" t="s">
         <v>122</v>
       </c>
-      <c r="E11" s="104" t="s">
+      <c r="E11" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="F11" s="104" t="s">
+      <c r="F11" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="G11" s="104" t="s">
+      <c r="G11" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="H11" s="104" t="s">
+      <c r="H11" s="107" t="s">
         <v>138</v>
       </c>
-      <c r="I11" s="105" t="s">
+      <c r="I11" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="J11" s="106" t="n">
+      <c r="J11" s="109" t="n">
         <v>8</v>
       </c>
-      <c r="K11" s="105" t="s">
+      <c r="K11" s="108" t="s">
         <v>110</v>
       </c>
-      <c r="L11" s="104" t="s">
+      <c r="L11" s="107" t="s">
         <v>112</v>
       </c>
-      <c r="M11" s="104" t="s">
+      <c r="M11" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="N11" s="117" t="n">
+      <c r="N11" s="120" t="n">
         <v>24</v>
       </c>
-      <c r="O11" s="118" t="s">
+      <c r="O11" s="121" t="s">
         <v>139</v>
       </c>
-      <c r="P11" s="106" t="s">
+      <c r="P11" s="109" t="s">
         <v>140</v>
       </c>
-      <c r="Q11" s="107" t="s">
+      <c r="Q11" s="110" t="s">
         <v>141</v>
       </c>
-      <c r="R11" s="107" t="s">
+      <c r="R11" s="110" t="s">
         <v>141</v>
       </c>
-      <c r="S11" s="115" t="s">
+      <c r="S11" s="118" t="s">
         <v>142</v>
       </c>
-      <c r="T11" s="106" t="s">
+      <c r="T11" s="109" t="s">
         <v>151</v>
       </c>
-      <c r="U11" s="106" t="s">
+      <c r="U11" s="109" t="s">
         <v>144</v>
       </c>
-      <c r="V11" s="105" t="s">
+      <c r="V11" s="108" t="s">
         <v>145</v>
       </c>
-      <c r="W11" s="107" t="s">
+      <c r="W11" s="110" t="s">
         <v>146</v>
       </c>
-      <c r="X11" s="106" t="s">
+      <c r="X11" s="109" t="s">
         <v>115</v>
       </c>
-      <c r="Y11" s="116" t="s">
+      <c r="Y11" s="119" t="s">
         <v>116</v>
       </c>
-      <c r="Z11" s="109"/>
-      <c r="AA11" s="110"/>
+      <c r="Z11" s="112"/>
+      <c r="AA11" s="113"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.5" outlineLevel="0" r="12">
-      <c r="A12" s="112"/>
-      <c r="B12" s="113"/>
-      <c r="C12" s="113"/>
-      <c r="D12" s="113"/>
-      <c r="E12" s="113"/>
-      <c r="F12" s="113"/>
-      <c r="G12" s="113"/>
-      <c r="H12" s="113"/>
-      <c r="I12" s="113"/>
-      <c r="J12" s="113"/>
-      <c r="K12" s="113"/>
-      <c r="L12" s="113"/>
-      <c r="M12" s="113"/>
-      <c r="N12" s="113"/>
-      <c r="O12" s="113"/>
-      <c r="P12" s="113"/>
-      <c r="Q12" s="113"/>
-      <c r="R12" s="113"/>
-      <c r="S12" s="113"/>
-      <c r="T12" s="113"/>
-      <c r="U12" s="113"/>
-      <c r="V12" s="113"/>
-      <c r="W12" s="113"/>
-      <c r="X12" s="113"/>
-      <c r="Y12" s="113"/>
-      <c r="Z12" s="113"/>
-      <c r="AA12" s="114"/>
+      <c r="A12" s="115"/>
+      <c r="B12" s="116"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="116"/>
+      <c r="H12" s="116"/>
+      <c r="I12" s="116"/>
+      <c r="J12" s="116"/>
+      <c r="K12" s="116"/>
+      <c r="L12" s="116"/>
+      <c r="M12" s="116"/>
+      <c r="N12" s="116"/>
+      <c r="O12" s="116"/>
+      <c r="P12" s="116"/>
+      <c r="Q12" s="116"/>
+      <c r="R12" s="116"/>
+      <c r="S12" s="116"/>
+      <c r="T12" s="116"/>
+      <c r="U12" s="116"/>
+      <c r="V12" s="116"/>
+      <c r="W12" s="116"/>
+      <c r="X12" s="116"/>
+      <c r="Y12" s="116"/>
+      <c r="Z12" s="116"/>
+      <c r="AA12" s="117"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5908,194 +5992,194 @@
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="122" t="s">
         <v>152</v>
       </c>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="G3" s="120"/>
-      <c r="H3" s="120"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="33.95" outlineLevel="0" r="4"/>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39" outlineLevel="0" r="5" s="100">
-      <c r="A5" s="97" t="s">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39" outlineLevel="0" r="5" s="103">
+      <c r="A5" s="100" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="124" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="97" t="s">
+      <c r="C5" s="100" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="100" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="100" t="s">
         <v>153</v>
       </c>
-      <c r="F5" s="97" t="s">
+      <c r="F5" s="100" t="s">
         <v>154</v>
       </c>
-      <c r="G5" s="97" t="s">
+      <c r="G5" s="100" t="s">
         <v>155</v>
       </c>
-      <c r="H5" s="97" t="s">
+      <c r="H5" s="100" t="s">
         <v>156</v>
       </c>
-      <c r="I5" s="97" t="s">
+      <c r="I5" s="100" t="s">
         <v>157</v>
       </c>
-      <c r="J5" s="98" t="s">
+      <c r="J5" s="101" t="s">
         <v>158</v>
       </c>
-      <c r="K5" s="98" t="s">
+      <c r="K5" s="101" t="s">
         <v>159</v>
       </c>
-      <c r="L5" s="98" t="s">
+      <c r="L5" s="101" t="s">
         <v>160</v>
       </c>
-      <c r="M5" s="98" t="s">
+      <c r="M5" s="101" t="s">
         <v>101</v>
       </c>
-      <c r="N5" s="98" t="s">
+      <c r="N5" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="O5" s="97" t="s">
+      <c r="O5" s="100" t="s">
         <v>103</v>
       </c>
-      <c r="P5" s="99"/>
+      <c r="P5" s="102"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
-      <c r="A6" s="101"/>
-      <c r="B6" s="101"/>
-      <c r="C6" s="102"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="102"/>
-      <c r="I6" s="102"/>
-      <c r="J6" s="102"/>
-      <c r="K6" s="102"/>
-      <c r="L6" s="102"/>
-      <c r="M6" s="102"/>
-      <c r="N6" s="102"/>
-      <c r="O6" s="102"/>
-      <c r="P6" s="103"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="111">
-      <c r="A7" s="104" t="s">
+      <c r="A6" s="104"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="105"/>
+      <c r="J6" s="105"/>
+      <c r="K6" s="105"/>
+      <c r="L6" s="105"/>
+      <c r="M6" s="105"/>
+      <c r="N6" s="105"/>
+      <c r="O6" s="105"/>
+      <c r="P6" s="106"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="114">
+      <c r="A7" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="122" t="s">
+      <c r="B7" s="125" t="s">
         <v>161</v>
       </c>
-      <c r="C7" s="105" t="s">
+      <c r="C7" s="108" t="s">
         <v>162</v>
       </c>
-      <c r="D7" s="104" t="s">
+      <c r="D7" s="107" t="s">
         <v>163</v>
       </c>
-      <c r="E7" s="104" t="s">
+      <c r="E7" s="107" t="s">
         <v>164</v>
       </c>
-      <c r="F7" s="104" t="s">
+      <c r="F7" s="107" t="s">
         <v>165</v>
       </c>
-      <c r="G7" s="104" t="s">
+      <c r="G7" s="107" t="s">
         <v>166</v>
       </c>
-      <c r="H7" s="104" t="s">
+      <c r="H7" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="I7" s="104" t="s">
+      <c r="I7" s="107" t="s">
         <v>168</v>
       </c>
-      <c r="J7" s="106" t="s">
+      <c r="J7" s="109" t="s">
         <v>169</v>
       </c>
-      <c r="K7" s="106" t="s">
+      <c r="K7" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="L7" s="107" t="s">
+      <c r="L7" s="110" t="s">
         <v>170</v>
       </c>
-      <c r="M7" s="106" t="s">
+      <c r="M7" s="109" t="s">
         <v>171</v>
       </c>
-      <c r="N7" s="116" t="s">
+      <c r="N7" s="119" t="s">
         <v>116</v>
       </c>
-      <c r="O7" s="123" t="s">
+      <c r="O7" s="126" t="s">
         <v>172</v>
       </c>
-      <c r="P7" s="110"/>
+      <c r="P7" s="113"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="8">
-      <c r="A8" s="104" t="s">
+      <c r="A8" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="122" t="s">
+      <c r="B8" s="125" t="s">
         <v>173</v>
       </c>
-      <c r="C8" s="105" t="s">
+      <c r="C8" s="108" t="s">
         <v>174</v>
       </c>
-      <c r="D8" s="104" t="s">
+      <c r="D8" s="107" t="s">
         <v>175</v>
       </c>
-      <c r="E8" s="124" t="s">
+      <c r="E8" s="127" t="s">
         <v>164</v>
       </c>
-      <c r="F8" s="104" t="s">
+      <c r="F8" s="107" t="s">
         <v>165</v>
       </c>
-      <c r="G8" s="124" t="s">
+      <c r="G8" s="127" t="s">
         <v>166</v>
       </c>
-      <c r="H8" s="124" t="s">
+      <c r="H8" s="127" t="s">
         <v>167</v>
       </c>
-      <c r="I8" s="104" t="s">
+      <c r="I8" s="107" t="s">
         <v>168</v>
       </c>
-      <c r="J8" s="106" t="s">
+      <c r="J8" s="109" t="s">
         <v>169</v>
       </c>
-      <c r="K8" s="106" t="s">
+      <c r="K8" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="L8" s="107" t="s">
+      <c r="L8" s="110" t="s">
         <v>170</v>
       </c>
-      <c r="M8" s="106" t="s">
+      <c r="M8" s="109" t="s">
         <v>171</v>
       </c>
-      <c r="N8" s="116" t="s">
+      <c r="N8" s="119" t="s">
         <v>116</v>
       </c>
-      <c r="O8" s="123" t="s">
+      <c r="O8" s="126" t="s">
         <v>172</v>
       </c>
-      <c r="P8" s="110"/>
+      <c r="P8" s="113"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.5" outlineLevel="0" r="9">
-      <c r="A9" s="112"/>
-      <c r="B9" s="112"/>
-      <c r="C9" s="113"/>
-      <c r="D9" s="113"/>
-      <c r="E9" s="113"/>
-      <c r="F9" s="113"/>
-      <c r="G9" s="113"/>
-      <c r="H9" s="113"/>
-      <c r="I9" s="113"/>
-      <c r="J9" s="113"/>
-      <c r="K9" s="113"/>
-      <c r="L9" s="113"/>
-      <c r="M9" s="113"/>
-      <c r="N9" s="113"/>
-      <c r="O9" s="113"/>
-      <c r="P9" s="114"/>
+      <c r="A9" s="115"/>
+      <c r="B9" s="115"/>
+      <c r="C9" s="116"/>
+      <c r="D9" s="116"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="116"/>
+      <c r="G9" s="116"/>
+      <c r="H9" s="116"/>
+      <c r="I9" s="116"/>
+      <c r="J9" s="116"/>
+      <c r="K9" s="116"/>
+      <c r="L9" s="116"/>
+      <c r="M9" s="116"/>
+      <c r="N9" s="116"/>
+      <c r="O9" s="116"/>
+      <c r="P9" s="117"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>